<commit_message>
fixed stack too deep problem by removing school name method and repositioned buttons
</commit_message>
<xml_diff>
--- a/children.xlsx
+++ b/children.xlsx
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -79,7 +79,8 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="11.88988764044944"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="6.389887640449439"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="16.28988764044944"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.68988764044944"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.489887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -115,6 +116,11 @@
       </c>
       <c r="G1" s="0" t="inlineStr">
         <is>
+          <t>School</t>
+        </is>
+      </c>
+      <c r="H1" s="0" t="inlineStr">
+        <is>
           <t>Programs</t>
         </is>
       </c>
@@ -144,7 +150,12 @@
           <t>Jessica Bac</t>
         </is>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H2" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -173,7 +184,12 @@
           <t>Gayle Barton</t>
         </is>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H3" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -202,7 +218,12 @@
           <t>Gayle Barton</t>
         </is>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H4" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -231,7 +252,12 @@
           <t>Jarvis Beatty</t>
         </is>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -260,7 +286,12 @@
           <t>Jarvis Beatty</t>
         </is>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -289,7 +320,12 @@
           <t>Lera Braun</t>
         </is>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H7" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -318,7 +354,12 @@
           <t>Lera Braun</t>
         </is>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -347,7 +388,12 @@
           <t>Markita Clark</t>
         </is>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H9" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -376,7 +422,12 @@
           <t>Markita Clark</t>
         </is>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H10" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -405,7 +456,12 @@
           <t>Markita Clark</t>
         </is>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H11" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -434,7 +490,12 @@
           <t>Macie Deckow</t>
         </is>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H12" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -463,7 +524,12 @@
           <t>Macie Deckow</t>
         </is>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H13" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -492,7 +558,12 @@
           <t>Marcia Gregory</t>
         </is>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H14" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -521,7 +592,12 @@
           <t>Kattie Hamill</t>
         </is>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H15" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -550,7 +626,12 @@
           <t>Kattie Hamill</t>
         </is>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H16" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -579,7 +660,12 @@
           <t>Kara Hand</t>
         </is>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H17" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -608,7 +694,12 @@
           <t>Kara Hand</t>
         </is>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H18" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -637,7 +728,12 @@
           <t>Susan Gormley</t>
         </is>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H19" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -666,7 +762,12 @@
           <t>Rasheedah Jefferson</t>
         </is>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H20" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -695,7 +796,12 @@
           <t>Susan Gormley</t>
         </is>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="G21" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H21" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -724,7 +830,12 @@
           <t>Rasheedah Jefferson</t>
         </is>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="G22" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H22" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -753,7 +864,12 @@
           <t>Rasheedah Jefferson</t>
         </is>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="G23" s="0" t="inlineStr">
+        <is>
+          <t>Penn Hills Middle School</t>
+        </is>
+      </c>
+      <c r="H23" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -782,7 +898,12 @@
           <t>Show Guardian</t>
         </is>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G24" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H24" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -811,7 +932,12 @@
           <t>Verona Koss</t>
         </is>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H25" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -840,7 +966,12 @@
           <t>Verona Koss</t>
         </is>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G26" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H26" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -869,7 +1000,12 @@
           <t>Ronny Kreiger</t>
         </is>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="G27" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H27" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -898,7 +1034,12 @@
           <t>Ronny Kreiger</t>
         </is>
       </c>
-      <c r="G28" s="0" t="n">
+      <c r="G28" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H28" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -927,7 +1068,12 @@
           <t>Arturo Lakin</t>
         </is>
       </c>
-      <c r="G29" s="0" t="n">
+      <c r="G29" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H29" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -956,7 +1102,12 @@
           <t>Arturo Lakin</t>
         </is>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="G30" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H30" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -985,7 +1136,12 @@
           <t>Foster Legros</t>
         </is>
       </c>
-      <c r="G31" s="0" t="n">
+      <c r="G31" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H31" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1014,7 +1170,12 @@
           <t>Foster Legros</t>
         </is>
       </c>
-      <c r="G32" s="0" t="n">
+      <c r="G32" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H32" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1043,7 +1204,12 @@
           <t>Heloise McDermott</t>
         </is>
       </c>
-      <c r="G33" s="0" t="n">
+      <c r="G33" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H33" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1072,7 +1238,12 @@
           <t>Heloise McDermott</t>
         </is>
       </c>
-      <c r="G34" s="0" t="n">
+      <c r="G34" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H34" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1101,7 +1272,12 @@
           <t>Heloise McDermott</t>
         </is>
       </c>
-      <c r="G35" s="0" t="n">
+      <c r="G35" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H35" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1130,7 +1306,12 @@
           <t>Daija Mertz</t>
         </is>
       </c>
-      <c r="G36" s="0" t="n">
+      <c r="G36" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H36" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1159,7 +1340,12 @@
           <t>Daija Mertz</t>
         </is>
       </c>
-      <c r="G37" s="0" t="n">
+      <c r="G37" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H37" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1188,7 +1374,12 @@
           <t>Dillan Quigley</t>
         </is>
       </c>
-      <c r="G38" s="0" t="n">
+      <c r="G38" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H38" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1217,7 +1408,12 @@
           <t>Dillan Quigley</t>
         </is>
       </c>
-      <c r="G39" s="0" t="n">
+      <c r="G39" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H39" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1246,7 +1442,12 @@
           <t>Isabell Reichel</t>
         </is>
       </c>
-      <c r="G40" s="0" t="n">
+      <c r="G40" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H40" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1275,7 +1476,12 @@
           <t>Isabell Reichel</t>
         </is>
       </c>
-      <c r="G41" s="0" t="n">
+      <c r="G41" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H41" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1304,7 +1510,12 @@
           <t>Adaline Reichert</t>
         </is>
       </c>
-      <c r="G42" s="0" t="n">
+      <c r="G42" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H42" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1333,7 +1544,12 @@
           <t>Adaline Reichert</t>
         </is>
       </c>
-      <c r="G43" s="0" t="n">
+      <c r="G43" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H43" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1362,7 +1578,12 @@
           <t>Aniyah Reinger</t>
         </is>
       </c>
-      <c r="G44" s="0" t="n">
+      <c r="G44" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H44" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1391,7 +1612,12 @@
           <t>Aniyah Reinger</t>
         </is>
       </c>
-      <c r="G45" s="0" t="n">
+      <c r="G45" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H45" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1420,7 +1646,12 @@
           <t>Heloise McDermott</t>
         </is>
       </c>
-      <c r="G46" s="0" t="n">
+      <c r="G46" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H46" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1449,7 +1680,12 @@
           <t>Bernice Stoltenberg</t>
         </is>
       </c>
-      <c r="G47" s="0" t="n">
+      <c r="G47" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H47" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1478,7 +1714,12 @@
           <t>Bernice Stoltenberg</t>
         </is>
       </c>
-      <c r="G48" s="0" t="n">
+      <c r="G48" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H48" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1507,7 +1748,12 @@
           <t>Ali Stroman</t>
         </is>
       </c>
-      <c r="G49" s="0" t="n">
+      <c r="G49" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H49" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1536,7 +1782,12 @@
           <t>Ali Stroman</t>
         </is>
       </c>
-      <c r="G50" s="0" t="n">
+      <c r="G50" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H50" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1565,7 +1816,12 @@
           <t>Abdul Ullrich</t>
         </is>
       </c>
-      <c r="G51" s="0" t="n">
+      <c r="G51" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H51" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1594,7 +1850,12 @@
           <t>Abdul Ullrich</t>
         </is>
       </c>
-      <c r="G52" s="0" t="n">
+      <c r="G52" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H52" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1623,7 +1884,12 @@
           <t>Margaret Volkman</t>
         </is>
       </c>
-      <c r="G53" s="0" t="n">
+      <c r="G53" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H53" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1652,7 +1918,12 @@
           <t>Margaret Volkman</t>
         </is>
       </c>
-      <c r="G54" s="0" t="n">
+      <c r="G54" s="0" t="inlineStr">
+        <is>
+          <t>Sunnyside</t>
+        </is>
+      </c>
+      <c r="H54" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel download feature for programs
</commit_message>
<xml_diff>
--- a/children.xlsx
+++ b/children.xlsx
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -79,8 +79,11 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="11.88988764044944"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="6.389887640449439"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="16.28988764044944"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.68988764044944"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.88988764044944"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.989887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -116,12 +119,27 @@
       </c>
       <c r="G1" s="0" t="inlineStr">
         <is>
-          <t>School</t>
+          <t>Programs</t>
         </is>
       </c>
       <c r="H1" s="0" t="inlineStr">
         <is>
-          <t>Programs</t>
+          <t>Homework</t>
+        </is>
+      </c>
+      <c r="I1" s="0" t="inlineStr">
+        <is>
+          <t>Literacy</t>
+        </is>
+      </c>
+      <c r="J1" s="0" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
+      <c r="K1" s="0" t="inlineStr">
+        <is>
+          <t>Reading Specialist</t>
         </is>
       </c>
     </row>
@@ -150,13 +168,20 @@
           <t>Jessica Bac</t>
         </is>
       </c>
-      <c r="G2" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G2" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -177,19 +202,26 @@
         <v>39423.0</v>
       </c>
       <c r="E3" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
           <t>Gayle Barton</t>
         </is>
       </c>
-      <c r="G3" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G3" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -218,12 +250,19 @@
           <t>Gayle Barton</t>
         </is>
       </c>
-      <c r="G4" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G4" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -252,12 +291,19 @@
           <t>Jarvis Beatty</t>
         </is>
       </c>
-      <c r="G5" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G5" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -286,12 +332,19 @@
           <t>Jarvis Beatty</t>
         </is>
       </c>
-      <c r="G6" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G6" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -320,12 +373,19 @@
           <t>Lera Braun</t>
         </is>
       </c>
-      <c r="G7" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G7" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -354,12 +414,19 @@
           <t>Lera Braun</t>
         </is>
       </c>
-      <c r="G8" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G8" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -388,13 +455,20 @@
           <t>Markita Clark</t>
         </is>
       </c>
-      <c r="G9" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G9" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="10">
@@ -422,13 +496,20 @@
           <t>Markita Clark</t>
         </is>
       </c>
-      <c r="G10" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G10" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -456,13 +537,20 @@
           <t>Markita Clark</t>
         </is>
       </c>
-      <c r="G11" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G11" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>3</v>
+        <v>40</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="12">
@@ -490,12 +578,19 @@
           <t>Macie Deckow</t>
         </is>
       </c>
-      <c r="G12" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G12" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -524,12 +619,19 @@
           <t>Macie Deckow</t>
         </is>
       </c>
-      <c r="G13" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G13" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -558,13 +660,20 @@
           <t>Marcia Gregory</t>
         </is>
       </c>
-      <c r="G14" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G14" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -592,12 +701,19 @@
           <t>Kattie Hamill</t>
         </is>
       </c>
-      <c r="G15" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G15" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -626,12 +742,19 @@
           <t>Kattie Hamill</t>
         </is>
       </c>
-      <c r="G16" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G16" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -660,12 +783,19 @@
           <t>Kara Hand</t>
         </is>
       </c>
-      <c r="G17" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G17" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -694,12 +824,19 @@
           <t>Kara Hand</t>
         </is>
       </c>
-      <c r="G18" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G18" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -728,13 +865,20 @@
           <t>Susan Gormley</t>
         </is>
       </c>
-      <c r="G19" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G19" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="20">
@@ -762,13 +906,20 @@
           <t>Rasheedah Jefferson</t>
         </is>
       </c>
-      <c r="G20" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G20" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -796,13 +947,20 @@
           <t>Susan Gormley</t>
         </is>
       </c>
-      <c r="G21" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G21" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -830,13 +988,20 @@
           <t>Rasheedah Jefferson</t>
         </is>
       </c>
-      <c r="G22" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G22" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -864,13 +1029,20 @@
           <t>Rasheedah Jefferson</t>
         </is>
       </c>
-      <c r="G23" s="0" t="inlineStr">
-        <is>
-          <t>Penn Hills Middle School</t>
-        </is>
+      <c r="G23" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="H23" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -898,12 +1070,19 @@
           <t>Show Guardian</t>
         </is>
       </c>
-      <c r="G24" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G24" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -932,12 +1111,19 @@
           <t>Verona Koss</t>
         </is>
       </c>
-      <c r="G25" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G25" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -966,12 +1152,19 @@
           <t>Verona Koss</t>
         </is>
       </c>
-      <c r="G26" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G26" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1000,12 +1193,19 @@
           <t>Ronny Kreiger</t>
         </is>
       </c>
-      <c r="G27" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G27" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1034,12 +1234,19 @@
           <t>Ronny Kreiger</t>
         </is>
       </c>
-      <c r="G28" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G28" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1068,12 +1275,19 @@
           <t>Arturo Lakin</t>
         </is>
       </c>
-      <c r="G29" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G29" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1102,12 +1316,19 @@
           <t>Arturo Lakin</t>
         </is>
       </c>
-      <c r="G30" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G30" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1136,12 +1357,19 @@
           <t>Foster Legros</t>
         </is>
       </c>
-      <c r="G31" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G31" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1170,12 +1398,19 @@
           <t>Foster Legros</t>
         </is>
       </c>
-      <c r="G32" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G32" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1204,12 +1439,19 @@
           <t>Heloise McDermott</t>
         </is>
       </c>
-      <c r="G33" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G33" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1238,12 +1480,19 @@
           <t>Heloise McDermott</t>
         </is>
       </c>
-      <c r="G34" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G34" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1272,12 +1521,19 @@
           <t>Heloise McDermott</t>
         </is>
       </c>
-      <c r="G35" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G35" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1306,12 +1562,19 @@
           <t>Daija Mertz</t>
         </is>
       </c>
-      <c r="G36" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G36" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1340,12 +1603,19 @@
           <t>Daija Mertz</t>
         </is>
       </c>
-      <c r="G37" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G37" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1374,12 +1644,19 @@
           <t>Dillan Quigley</t>
         </is>
       </c>
-      <c r="G38" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G38" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1408,12 +1685,19 @@
           <t>Dillan Quigley</t>
         </is>
       </c>
-      <c r="G39" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G39" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1442,12 +1726,19 @@
           <t>Isabell Reichel</t>
         </is>
       </c>
-      <c r="G40" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G40" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1476,12 +1767,19 @@
           <t>Isabell Reichel</t>
         </is>
       </c>
-      <c r="G41" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G41" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1510,12 +1808,19 @@
           <t>Adaline Reichert</t>
         </is>
       </c>
-      <c r="G42" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G42" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1544,12 +1849,19 @@
           <t>Adaline Reichert</t>
         </is>
       </c>
-      <c r="G43" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G43" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1578,12 +1890,19 @@
           <t>Aniyah Reinger</t>
         </is>
       </c>
-      <c r="G44" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G44" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1612,12 +1931,19 @@
           <t>Aniyah Reinger</t>
         </is>
       </c>
-      <c r="G45" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G45" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1646,12 +1972,19 @@
           <t>Heloise McDermott</t>
         </is>
       </c>
-      <c r="G46" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G46" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1680,12 +2013,19 @@
           <t>Bernice Stoltenberg</t>
         </is>
       </c>
-      <c r="G47" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G47" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1714,12 +2054,19 @@
           <t>Bernice Stoltenberg</t>
         </is>
       </c>
-      <c r="G48" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G48" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1748,12 +2095,19 @@
           <t>Ali Stroman</t>
         </is>
       </c>
-      <c r="G49" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G49" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1782,12 +2136,19 @@
           <t>Ali Stroman</t>
         </is>
       </c>
-      <c r="G50" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G50" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1816,12 +2177,19 @@
           <t>Abdul Ullrich</t>
         </is>
       </c>
-      <c r="G51" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G51" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1850,12 +2218,19 @@
           <t>Abdul Ullrich</t>
         </is>
       </c>
-      <c r="G52" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G52" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1884,12 +2259,19 @@
           <t>Margaret Volkman</t>
         </is>
       </c>
-      <c r="G53" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G53" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1918,12 +2300,19 @@
           <t>Margaret Volkman</t>
         </is>
       </c>
-      <c r="G54" s="0" t="inlineStr">
-        <is>
-          <t>Sunnyside</t>
-        </is>
+      <c r="G54" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel downloads updated to include physical and hands on activity
</commit_message>
<xml_diff>
--- a/children.xlsx
+++ b/children.xlsx
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -84,6 +84,8 @@
     <col min="9" max="9" bestFit="true" customWidth="true" width="5.289887640449439"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="11.88988764044944"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="12.989887640449439"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.78988764044944"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="14.08988764044944"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -142,6 +144,16 @@
           <t>Reading Specialist</t>
         </is>
       </c>
+      <c r="L1" s="0" t="inlineStr">
+        <is>
+          <t>Physical Activity</t>
+        </is>
+      </c>
+      <c r="M1" s="0" t="inlineStr">
+        <is>
+          <t>Hands On Time</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="n">
@@ -183,6 +195,12 @@
       <c r="K2" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="n">
@@ -224,6 +242,12 @@
       <c r="K3" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="n">
@@ -265,6 +289,12 @@
       <c r="K4" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="n">
@@ -306,6 +336,12 @@
       <c r="K5" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="n">
@@ -347,6 +383,12 @@
       <c r="K6" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="n">
@@ -388,6 +430,12 @@
       <c r="K7" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="n">
@@ -429,6 +477,12 @@
       <c r="K8" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="n">
@@ -459,16 +513,22 @@
         <v>3</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I9" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="L9" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="J9" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>30</v>
+      <c r="M9" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="10">
@@ -500,16 +560,22 @@
         <v>3</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I10" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="L10" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="J10" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>0</v>
+      <c r="M10" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="11">
@@ -541,16 +607,22 @@
         <v>3</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="I11" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="K11" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="L11" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="K11" s="0" t="n">
-        <v>15</v>
+      <c r="M11" s="0" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="12">
@@ -593,6 +665,12 @@
       <c r="K12" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="n">
@@ -634,6 +712,12 @@
       <c r="K13" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="n">
@@ -675,6 +759,12 @@
       <c r="K14" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="n">
@@ -716,6 +806,12 @@
       <c r="K15" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="n">
@@ -757,6 +853,12 @@
       <c r="K16" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="n">
@@ -798,6 +900,12 @@
       <c r="K17" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="n">
@@ -839,6 +947,12 @@
       <c r="K18" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="n">
@@ -872,13 +986,19 @@
         <v>15</v>
       </c>
       <c r="I19" s="0" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K19" s="0" t="n">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="20">
@@ -921,6 +1041,12 @@
       <c r="K20" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="n">
@@ -962,6 +1088,12 @@
       <c r="K21" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="n">
@@ -1003,6 +1135,12 @@
       <c r="K22" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="n">
@@ -1044,6 +1182,12 @@
       <c r="K23" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="n">
@@ -1085,6 +1229,12 @@
       <c r="K24" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="n">
@@ -1126,6 +1276,12 @@
       <c r="K25" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="n">
@@ -1167,6 +1323,12 @@
       <c r="K26" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="n">
@@ -1208,6 +1370,12 @@
       <c r="K27" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="n">
@@ -1249,6 +1417,12 @@
       <c r="K28" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="n">
@@ -1290,6 +1464,12 @@
       <c r="K29" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="n">
@@ -1331,6 +1511,12 @@
       <c r="K30" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="n">
@@ -1372,6 +1558,12 @@
       <c r="K31" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="n">
@@ -1413,6 +1605,12 @@
       <c r="K32" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="n">
@@ -1454,6 +1652,12 @@
       <c r="K33" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="n">
@@ -1495,6 +1699,12 @@
       <c r="K34" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="n">
@@ -1536,6 +1746,12 @@
       <c r="K35" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="n">
@@ -1577,6 +1793,12 @@
       <c r="K36" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="n">
@@ -1618,6 +1840,12 @@
       <c r="K37" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="n">
@@ -1659,6 +1887,12 @@
       <c r="K38" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="n">
@@ -1700,6 +1934,12 @@
       <c r="K39" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="n">
@@ -1741,6 +1981,12 @@
       <c r="K40" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="n">
@@ -1782,6 +2028,12 @@
       <c r="K41" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="n">
@@ -1823,6 +2075,12 @@
       <c r="K42" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="n">
@@ -1864,6 +2122,12 @@
       <c r="K43" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="n">
@@ -1905,6 +2169,12 @@
       <c r="K44" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="n">
@@ -1946,6 +2216,12 @@
       <c r="K45" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="n">
@@ -1987,6 +2263,12 @@
       <c r="K46" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="n">
@@ -2028,6 +2310,12 @@
       <c r="K47" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M47" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="n">
@@ -2069,6 +2357,12 @@
       <c r="K48" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M48" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="n">
@@ -2110,6 +2404,12 @@
       <c r="K49" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M49" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="n">
@@ -2151,6 +2451,12 @@
       <c r="K50" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M50" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="n">
@@ -2192,6 +2498,12 @@
       <c r="K51" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M51" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="n">
@@ -2233,6 +2545,12 @@
       <c r="K52" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="n">
@@ -2274,6 +2592,12 @@
       <c r="K53" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="L53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M53" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="n">
@@ -2313,6 +2637,12 @@
         <v>0</v>
       </c>
       <c r="K54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M54" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>